<commit_message>
Added error handling for retrieving file properties for multiple parts
</commit_message>
<xml_diff>
--- a/custom_properties.xlsx
+++ b/custom_properties.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB19"/>
+  <dimension ref="A1:AB53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2396,6 +2396,3476 @@
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr"/>
     </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>LS1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Bumper Shell Interface</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z20" t="inlineStr"/>
+      <c r="AA20" t="inlineStr"/>
+      <c r="AB20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>LS2</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Base-Shell Breakout (From Main Body Components to Shell Baseplate)</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z21" t="inlineStr"/>
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>LS3</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Rear Aux (Kernel Module to Rear Fan)</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z22" t="inlineStr"/>
+      <c r="AA22" t="inlineStr"/>
+      <c r="AB22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>LS4a</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>NVR (Kernel Module to NVR)</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z23" t="inlineStr"/>
+      <c r="AA23" t="inlineStr"/>
+      <c r="AB23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>LS4b</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Front Aux (From Kernel Module to Speakers + Intake Fan)
+</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr"/>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z24" t="inlineStr"/>
+      <c r="AA24" t="inlineStr"/>
+      <c r="AB24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>LS5</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Kernel-Hat Link (From Top Enclosure Interface Plate to Kernel Module)</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z25" t="inlineStr"/>
+      <c r="AA25" t="inlineStr"/>
+      <c r="AB25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>LS6</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Lighting System (From Aether Module to Headlights)</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
+      <c r="AB26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>LS7</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Intrusion Subsystem (From DB9 Adapter to Intrusion Switches)</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr"/>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
+      <c r="AB27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SB1</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Scout Base Shell Link (From Shell Baseplate to Scout Base)</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr"/>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z28" t="inlineStr"/>
+      <c r="AA28" t="inlineStr"/>
+      <c r="AB28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SB2</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Scout Base Internals (From Scout Interface Plate to Internal Scout Components)</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr"/>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z29" t="inlineStr"/>
+      <c r="AA29" t="inlineStr"/>
+      <c r="AB29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>SB3a</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Bumper Shell Link (From Shell Baseplate to Bumper)</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr"/>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z30" t="inlineStr"/>
+      <c r="AA30" t="inlineStr"/>
+      <c r="AB30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>SB3b</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr"/>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>2D Lidar Link (From Shell Baseplate to 2D Lidar)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr"/>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z31" t="inlineStr"/>
+      <c r="AA31" t="inlineStr"/>
+      <c r="AB31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>SB4a</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Bumper Shell Link (Shell Baseplate to Bumper)</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z32" t="inlineStr"/>
+      <c r="AA32" t="inlineStr"/>
+      <c r="AB32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SB4b</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>IP Cam Link (From Shell Baseplate to IPCam)</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr"/>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z33" t="inlineStr"/>
+      <c r="AA33" t="inlineStr"/>
+      <c r="AB33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>SB5</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Bumper Internals (From Bumper Interface Plate to Internal Bumper Components)</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr"/>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z34" t="inlineStr"/>
+      <c r="AA34" t="inlineStr"/>
+      <c r="AB34" t="inlineStr"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>testpart</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Bumper Shell Interface</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr"/>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z35" t="inlineStr"/>
+      <c r="AA35" t="inlineStr"/>
+      <c r="AB35" t="inlineStr"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>TH1</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Top Hat Internals (From Top Hat Interface Plate to Internal Top Hat Components</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr"/>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z36" t="inlineStr"/>
+      <c r="AA36" t="inlineStr"/>
+      <c r="AB36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>LS1</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Bumper Shell Interface</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z37" t="inlineStr"/>
+      <c r="AA37" t="inlineStr"/>
+      <c r="AB37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>LS2</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Base-Shell Breakout (From Main Body Components to Shell Baseplate)</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr"/>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z38" t="inlineStr"/>
+      <c r="AA38" t="inlineStr"/>
+      <c r="AB38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>LS3</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Rear Aux (Kernel Module to Rear Fan)</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z39" t="inlineStr"/>
+      <c r="AA39" t="inlineStr"/>
+      <c r="AB39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>LS4a</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>NVR (Kernel Module to NVR)</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr"/>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z40" t="inlineStr"/>
+      <c r="AA40" t="inlineStr"/>
+      <c r="AB40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>LS4b</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Front Aux (From Kernel Module to Speakers + Intake Fan)
+</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr"/>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z41" t="inlineStr"/>
+      <c r="AA41" t="inlineStr"/>
+      <c r="AB41" t="inlineStr"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>LS5</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Kernel-Hat Link (From Top Enclosure Interface Plate to Kernel Module)</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr"/>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z42" t="inlineStr"/>
+      <c r="AA42" t="inlineStr"/>
+      <c r="AB42" t="inlineStr"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>LS6</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Lighting System (From Aether Module to Headlights)</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr"/>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z43" t="inlineStr"/>
+      <c r="AA43" t="inlineStr"/>
+      <c r="AB43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>LS7</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Intrusion Subsystem (From DB9 Adapter to Intrusion Switches)</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr"/>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X44" t="inlineStr"/>
+      <c r="Y44" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z44" t="inlineStr"/>
+      <c r="AA44" t="inlineStr"/>
+      <c r="AB44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>SB1</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Scout Base Shell Link (From Shell Baseplate to Scout Base)</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr"/>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z45" t="inlineStr"/>
+      <c r="AA45" t="inlineStr"/>
+      <c r="AB45" t="inlineStr"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SB2</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Scout Base Internals (From Scout Interface Plate to Internal Scout Components)</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O46" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr"/>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z46" t="inlineStr"/>
+      <c r="AA46" t="inlineStr"/>
+      <c r="AB46" t="inlineStr"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SB3a</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Bumper Shell Link (From Shell Baseplate to Bumper)</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O47" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr"/>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z47" t="inlineStr"/>
+      <c r="AA47" t="inlineStr"/>
+      <c r="AB47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>SB3b</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>2D Lidar Link (From Shell Baseplate to 2D Lidar)</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O48" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z48" t="inlineStr"/>
+      <c r="AA48" t="inlineStr"/>
+      <c r="AB48" t="inlineStr"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>SB4a</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Bumper Shell Link (Shell Baseplate to Bumper)</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O49" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z49" t="inlineStr"/>
+      <c r="AA49" t="inlineStr"/>
+      <c r="AB49" t="inlineStr"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>SB4b</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>IP Cam Link (From Shell Baseplate to IPCam)</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O50" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr"/>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z50" t="inlineStr"/>
+      <c r="AA50" t="inlineStr"/>
+      <c r="AB50" t="inlineStr"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>SB5</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Bumper Internals (From Bumper Interface Plate to Internal Bumper Components)</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O51" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z51" t="inlineStr"/>
+      <c r="AA51" t="inlineStr"/>
+      <c r="AB51" t="inlineStr"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>testpart</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Bumper Shell Interface</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O52" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr"/>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z52" t="inlineStr"/>
+      <c r="AA52" t="inlineStr"/>
+      <c r="AB52" t="inlineStr"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>TH1</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr"/>
+      <c r="D53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>Top Hat Internals (From Top Hat Interface Plate to Internal Top Hat Components</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>CBL</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O53" t="inlineStr">
+        <is>
+          <t>PC</t>
+        </is>
+      </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>MAKE</t>
+        </is>
+      </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr"/>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Z53" t="inlineStr"/>
+      <c r="AA53" t="inlineStr"/>
+      <c r="AB53" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added error handling and logfile generation with system date and time; modify_file_properties and set_file_properties now work properly with the generated custom_properties excel file
</commit_message>
<xml_diff>
--- a/custom_properties.xlsx
+++ b/custom_properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\OneDrive - Singapore University of Technology and Design\Desktop\Kabam Internship\Projects\Solidworks Wrapper Testing\pySldWrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADEBC92-4BDD-4FA8-BFA0-C4646F4B60A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B49B54B-1ED5-4C25-961A-D7E46F5D7323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
   <si>
     <t>Title</t>
   </si>
@@ -115,6 +115,9 @@
     <t>--</t>
   </si>
   <si>
+    <t>Material &lt;not specified&gt;</t>
+  </si>
+  <si>
     <t>CBL</t>
   </si>
   <si>
@@ -134,6 +137,10 @@
   </si>
   <si>
     <t>Rear Aux (Kernel Module to Rear Fan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Material &lt;not specified&gt;_x000D_
+</t>
   </si>
   <si>
     <t>LS4a</t>
@@ -149,25 +156,18 @@
 </t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>qe</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>Jjakdjak1235 24758823741</t>
-  </si>
-  <si>
-    <t>ad</t>
-  </si>
-  <si>
-    <t>qeqeqe</t>
+    <t xml:space="preserve">Material &lt;not specified&gt;_x000D_
+_x000D_
+</t>
+  </si>
+  <si>
+    <t>LS5</t>
+  </si>
+  <si>
+    <t>Kernel-Hat Link (From Top Enclosure Interface Plate to Kernel Module)</t>
+  </si>
+  <si>
+    <t>HALO</t>
   </si>
 </sst>
 </file>
@@ -531,17 +531,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="8" max="8" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -638,37 +638,22 @@
         <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G2" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" t="s">
-        <v>46</v>
-      </c>
-      <c r="L2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q2" t="s">
         <v>30</v>
@@ -688,43 +673,28 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" t="s">
         <v>34</v>
-      </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>30</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
       </c>
       <c r="Q3" t="s">
         <v>30</v>
@@ -744,43 +714,28 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
         <v>47</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q4" t="s">
         <v>30</v>
@@ -800,43 +755,28 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H5" t="s">
         <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" t="s">
-        <v>30</v>
-      </c>
-      <c r="N5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="Q5" t="s">
         <v>30</v>
@@ -856,57 +796,83 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="H6" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" t="s">
-        <v>30</v>
-      </c>
-      <c r="N6" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="O6" t="s">
+        <v>33</v>
+      </c>
+      <c r="P6" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" t="s">
+        <v>30</v>
+      </c>
+      <c r="U6" t="s">
+        <v>30</v>
+      </c>
+      <c r="W6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" t="s">
         <v>32</v>
       </c>
-      <c r="P6" t="s">
+      <c r="O7" t="s">
         <v>33</v>
       </c>
-      <c r="Q6" t="s">
-        <v>30</v>
-      </c>
-      <c r="S6" t="s">
-        <v>30</v>
-      </c>
-      <c r="U6" t="s">
-        <v>30</v>
-      </c>
-      <c r="W6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Y6" t="s">
+      <c r="P7" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="S7" t="s">
+        <v>30</v>
+      </c>
+      <c r="U7" t="s">
+        <v>30</v>
+      </c>
+      <c r="W7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y7" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added detection of excel files, extraction and comparison of excel file states
</commit_message>
<xml_diff>
--- a/custom_properties.xlsx
+++ b/custom_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\OneDrive - Singapore University of Technology and Design\Desktop\Kabam Internship\Projects\Solidworks Wrapper Testing\pySldWrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B49B54B-1ED5-4C25-961A-D7E46F5D7323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413579E0-5A1B-4265-A01F-4FBC08DE393A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="3945" windowWidth="21495" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Title</t>
   </si>
@@ -167,7 +167,16 @@
     <t>Kernel-Hat Link (From Top Enclosure Interface Plate to Kernel Module)</t>
   </si>
   <si>
-    <t>HALO</t>
+    <t>H</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>H2323</t>
+  </si>
+  <si>
+    <t>HALO111</t>
   </si>
 </sst>
 </file>
@@ -534,7 +543,7 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,8 +646,8 @@
       <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="F2" t="s">
-        <v>47</v>
+      <c r="F2">
+        <v>2323321</v>
       </c>
       <c r="G2" t="s">
         <v>31</v>
@@ -720,7 +729,7 @@
         <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G4" t="s">
         <v>39</v>
@@ -802,7 +811,7 @@
         <v>43</v>
       </c>
       <c r="F6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G6" t="s">
         <v>44</v>
@@ -843,7 +852,7 @@
         <v>46</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G7" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Integrated function for setting file properties into .py script, need to clean up script and document more things
</commit_message>
<xml_diff>
--- a/custom_properties.xlsx
+++ b/custom_properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\OneDrive - Singapore University of Technology and Design\Desktop\Kabam Internship\Projects\Solidworks Wrapper Testing\pySldWrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413579E0-5A1B-4265-A01F-4FBC08DE393A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FD8597-5CB9-40B5-97C8-5AD078A52720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="3945" windowWidth="21495" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>Title</t>
   </si>
@@ -115,9 +115,6 @@
     <t>--</t>
   </si>
   <si>
-    <t>Material &lt;not specified&gt;</t>
-  </si>
-  <si>
     <t>CBL</t>
   </si>
   <si>
@@ -137,10 +134,6 @@
   </si>
   <si>
     <t>Rear Aux (Kernel Module to Rear Fan)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Material &lt;not specified&gt;_x000D_
-</t>
   </si>
   <si>
     <t>LS4a</t>
@@ -156,27 +149,25 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Material &lt;not specified&gt;_x000D_
-_x000D_
-</t>
-  </si>
-  <si>
     <t>LS5</t>
   </si>
   <si>
     <t>Kernel-Hat Link (From Top Enclosure Interface Plate to Kernel Module)</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H2323</t>
-  </si>
-  <si>
-    <t>HALO111</t>
+    <t>a</t>
+  </si>
+  <si>
+    <t>bc</t>
+  </si>
+  <si>
+    <t>ad</t>
+  </si>
+  <si>
+    <t>qe</t>
+  </si>
+  <si>
+    <t>eeee</t>
   </si>
 </sst>
 </file>
@@ -543,7 +534,7 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,23 +637,23 @@
       <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="F2">
-        <v>2323321</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>123</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
         <v>31</v>
       </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
         <v>32</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>34</v>
       </c>
       <c r="Q2" t="s">
         <v>30</v>
@@ -682,28 +673,28 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
         <v>35</v>
       </c>
-      <c r="E3" t="s">
-        <v>36</v>
-      </c>
       <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3">
+        <v>123</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="O3" t="s">
         <v>32</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>33</v>
-      </c>
-      <c r="P3" t="s">
-        <v>34</v>
       </c>
       <c r="Q3" t="s">
         <v>30</v>
@@ -723,28 +714,28 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
       <c r="F4" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" t="s">
-        <v>39</v>
+        <v>47</v>
+      </c>
+      <c r="G4">
+        <v>123</v>
       </c>
       <c r="H4" t="s">
         <v>30</v>
       </c>
       <c r="I4" t="s">
+        <v>31</v>
+      </c>
+      <c r="O4" t="s">
         <v>32</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>33</v>
-      </c>
-      <c r="P4" t="s">
-        <v>34</v>
       </c>
       <c r="Q4" t="s">
         <v>30</v>
@@ -764,28 +755,28 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>47</v>
-      </c>
-      <c r="G5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5">
+        <v>123</v>
+      </c>
+      <c r="H5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" t="s">
         <v>31</v>
       </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="O5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>33</v>
-      </c>
-      <c r="P5" t="s">
-        <v>34</v>
       </c>
       <c r="Q5" t="s">
         <v>30</v>
@@ -805,28 +796,28 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="F6">
+        <v>111</v>
+      </c>
+      <c r="G6">
+        <v>123</v>
       </c>
       <c r="H6" t="s">
         <v>30</v>
       </c>
       <c r="I6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O6" t="s">
         <v>32</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>33</v>
-      </c>
-      <c r="P6" t="s">
-        <v>34</v>
       </c>
       <c r="Q6" t="s">
         <v>30</v>
@@ -846,28 +837,28 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
         <v>44</v>
       </c>
+      <c r="G7">
+        <v>123</v>
+      </c>
       <c r="H7" t="s">
         <v>30</v>
       </c>
       <c r="I7" t="s">
+        <v>31</v>
+      </c>
+      <c r="O7" t="s">
         <v>32</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>33</v>
-      </c>
-      <c r="P7" t="s">
-        <v>34</v>
       </c>
       <c r="Q7" t="s">
         <v>30</v>

</xml_diff>